<commit_message>
Updated WhatsApp bulk messenger with improved message handling and UI
</commit_message>
<xml_diff>
--- a/message_tracking/message_log.xlsx
+++ b/message_tracking/message_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2561,10 +2561,8 @@
           <t>2025-04-06 02:09:54</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>+919322612069</t>
-        </is>
+      <c r="B50" t="n">
+        <v>919322612069</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2582,6 +2580,1006 @@
         </is>
       </c>
       <c r="F50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-04-06 22:05:19</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>919322612069</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-04-06 22:05:51</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>91635348180</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Message: 
+Stacktrace:
+	GetHandleVerifier [0x00007FF68BA71F85+78133]
+	GetHandleVerifier [0x00007FF68BA71FE0+78224]
+	(No symbol) [0x00007FF68B8391BA]
+	(No symbol) [0x00007FF68B88F19D]
+	(No symbol) [0x00007FF68B88F44C]
+	(No symbol) [0x00007FF68B8E23D7]
+	(No symbol) [0x00007FF68B8B719F]
+	(No symbol) [0x00007FF68B8DF21F]
+	(No symbol) [0x00007FF68B8B6F33]
+	(No symbol) [0x00007FF68B880358]
+	(No symbol) [0x00007FF68B8810C3]
+	GetHandleVerifier [0x00007FF68BD3BAAD+3001437]
+	GetHandleVerifier [0x00007FF68BD35E92+2977858]
+	GetHandleVerifier [0x00007FF68BD5499D+3103565]
+	GetHandleVerifier [0x00007FF68BA8C81A+186826]
+	GetHandleVerifier [0x00007FF68BA9442F+218591]
+	GetHandleVerifier [0x00007FF68BA79DC4+110452]
+	GetHandleVerifier [0x00007FF68BA79F72+110882]
+	GetHandleVerifier [0x00007FF68BA603A9+5465]
+	BaseThreadInitThunk [0x00007FFD0A3EE8D7+23]
+	RtlUserThreadStart [0x00007FFD0B8DBF6C+44]
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-04-06 22:06:28</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>919322612069</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-04-06 22:06:39</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>916353481830</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-04-06 22:11:03</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>919322612069</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>yo</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Message: 
+Stacktrace:
+	GetHandleVerifier [0x00007FF68BA71F85+78133]
+	GetHandleVerifier [0x00007FF68BA71FE0+78224]
+	(No symbol) [0x00007FF68B8391BA]
+	(No symbol) [0x00007FF68B88F19D]
+	(No symbol) [0x00007FF68B88F44C]
+	(No symbol) [0x00007FF68B8E23D7]
+	(No symbol) [0x00007FF68B8B719F]
+	(No symbol) [0x00007FF68B8DF21F]
+	(No symbol) [0x00007FF68B8B6F33]
+	(No symbol) [0x00007FF68B880358]
+	(No symbol) [0x00007FF68B8810C3]
+	GetHandleVerifier [0x00007FF68BD3BAAD+3001437]
+	GetHandleVerifier [0x00007FF68BD35E92+2977858]
+	GetHandleVerifier [0x00007FF68BD5499D+3103565]
+	GetHandleVerifier [0x00007FF68BA8C81A+186826]
+	GetHandleVerifier [0x00007FF68BA9442F+218591]
+	GetHandleVerifier [0x00007FF68BA79DC4+110452]
+	GetHandleVerifier [0x00007FF68BA79F72+110882]
+	GetHandleVerifier [0x00007FF68BA603A9+5465]
+	BaseThreadInitThunk [0x00007FFD0A3EE8D7+23]
+	RtlUserThreadStart [0x00007FFD0B8DBF6C+44]
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-04-06 22:12:20</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>919322612069</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>yp</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Message: 
+Stacktrace:
+	GetHandleVerifier [0x00007FF68BA71F85+78133]
+	GetHandleVerifier [0x00007FF68BA71FE0+78224]
+	(No symbol) [0x00007FF68B8391BA]
+	(No symbol) [0x00007FF68B88F19D]
+	(No symbol) [0x00007FF68B88F44C]
+	(No symbol) [0x00007FF68B8E23D7]
+	(No symbol) [0x00007FF68B8B719F]
+	(No symbol) [0x00007FF68B8DF21F]
+	(No symbol) [0x00007FF68B8B6F33]
+	(No symbol) [0x00007FF68B880358]
+	(No symbol) [0x00007FF68B8810C3]
+	GetHandleVerifier [0x00007FF68BD3BAAD+3001437]
+	GetHandleVerifier [0x00007FF68BD35E92+2977858]
+	GetHandleVerifier [0x00007FF68BD5499D+3103565]
+	GetHandleVerifier [0x00007FF68BA8C81A+186826]
+	GetHandleVerifier [0x00007FF68BA9442F+218591]
+	GetHandleVerifier [0x00007FF68BA79DC4+110452]
+	GetHandleVerifier [0x00007FF68BA79F72+110882]
+	GetHandleVerifier [0x00007FF68BA603A9+5465]
+	BaseThreadInitThunk [0x00007FFD0A3EE8D7+23]
+	RtlUserThreadStart [0x00007FFD0B8DBF6C+44]
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-04-06 22:27:17</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>918849958013</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>cvfgh</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-04-06 22:37:05</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>918849958013</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Image: harshan_attar.png</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Message: 
+Stacktrace:
+	GetHandleVerifier [0x00007FF68BA71F85+78133]
+	GetHandleVerifier [0x00007FF68BA71FE0+78224]
+	(No symbol) [0x00007FF68B8391BA]
+	(No symbol) [0x00007FF68B88F19D]
+	(No symbol) [0x00007FF68B88F44C]
+	(No symbol) [0x00007FF68B8E23D7]
+	(No symbol) [0x00007FF68B8B719F]
+	(No symbol) [0x00007FF68B8DF21F]
+	(No symbol) [0x00007FF68B8B6F33]
+	(No symbol) [0x00007FF68B880358]
+	(No symbol) [0x00007FF68B8810C3]
+	GetHandleVerifier [0x00007FF68BD3BAAD+3001437]
+	GetHandleVerifier [0x00007FF68BD35E92+2977858]
+	GetHandleVerifier [0x00007FF68BD5499D+3103565]
+	GetHandleVerifier [0x00007FF68BA8C81A+186826]
+	GetHandleVerifier [0x00007FF68BA9442F+218591]
+	GetHandleVerifier [0x00007FF68BA79DC4+110452]
+	GetHandleVerifier [0x00007FF68BA79F72+110882]
+	GetHandleVerifier [0x00007FF68BA603A9+5465]
+	BaseThreadInitThunk [0x00007FFD0A3EE8D7+23]
+	RtlUserThreadStart [0x00007FFD0B8DBF6C+44]
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-04-06 22:38:16</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>918849958013</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Image: harshan_attar.png</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Message: 
+Stacktrace:
+	GetHandleVerifier [0x00007FF68BA71F85+78133]
+	GetHandleVerifier [0x00007FF68BA71FE0+78224]
+	(No symbol) [0x00007FF68B8391BA]
+	(No symbol) [0x00007FF68B88F19D]
+	(No symbol) [0x00007FF68B88F44C]
+	(No symbol) [0x00007FF68B8E23D7]
+	(No symbol) [0x00007FF68B8B719F]
+	(No symbol) [0x00007FF68B8DF21F]
+	(No symbol) [0x00007FF68B8B6F33]
+	(No symbol) [0x00007FF68B880358]
+	(No symbol) [0x00007FF68B8810C3]
+	GetHandleVerifier [0x00007FF68BD3BAAD+3001437]
+	GetHandleVerifier [0x00007FF68BD35E92+2977858]
+	GetHandleVerifier [0x00007FF68BD5499D+3103565]
+	GetHandleVerifier [0x00007FF68BA8C81A+186826]
+	GetHandleVerifier [0x00007FF68BA9442F+218591]
+	GetHandleVerifier [0x00007FF68BA79DC4+110452]
+	GetHandleVerifier [0x00007FF68BA79F72+110882]
+	GetHandleVerifier [0x00007FF68BA603A9+5465]
+	BaseThreadInitThunk [0x00007FFD0A3EE8D7+23]
+	RtlUserThreadStart [0x00007FFD0B8DBF6C+44]
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-04-06 22:50:09</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>918849958013</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Image: WhatsApp_Image_2024-08-31_at_11.24.11_ae2e19bd-removebg-preview.png</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Message: 
+Stacktrace:
+	GetHandleVerifier [0x00007FF68BA71F85+78133]
+	GetHandleVerifier [0x00007FF68BA71FE0+78224]
+	(No symbol) [0x00007FF68B8391BA]
+	(No symbol) [0x00007FF68B88F19D]
+	(No symbol) [0x00007FF68B88F44C]
+	(No symbol) [0x00007FF68B8E23D7]
+	(No symbol) [0x00007FF68B8B719F]
+	(No symbol) [0x00007FF68B8DF21F]
+	(No symbol) [0x00007FF68B8B6F33]
+	(No symbol) [0x00007FF68B880358]
+	(No symbol) [0x00007FF68B8810C3]
+	GetHandleVerifier [0x00007FF68BD3BAAD+3001437]
+	GetHandleVerifier [0x00007FF68BD35E92+2977858]
+	GetHandleVerifier [0x00007FF68BD5499D+3103565]
+	GetHandleVerifier [0x00007FF68BA8C81A+186826]
+	GetHandleVerifier [0x00007FF68BA9442F+218591]
+	GetHandleVerifier [0x00007FF68BA79DC4+110452]
+	GetHandleVerifier [0x00007FF68BA79F72+110882]
+	GetHandleVerifier [0x00007FF68BA603A9+5465]
+	BaseThreadInitThunk [0x00007FFD0A3EE8D7+23]
+	RtlUserThreadStart [0x00007FFD0B8DBF6C+44]
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-04-06 22:54:54</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>919322612069</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Image: 3853ec82-5d7e-4c3e-b266-2fca6f594a06.png</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Message: 
+Stacktrace:
+	GetHandleVerifier [0x00007FF68BA71F85+78133]
+	GetHandleVerifier [0x00007FF68BA71FE0+78224]
+	(No symbol) [0x00007FF68B8391BA]
+	(No symbol) [0x00007FF68B88F19D]
+	(No symbol) [0x00007FF68B88F44C]
+	(No symbol) [0x00007FF68B8E23D7]
+	(No symbol) [0x00007FF68B8B719F]
+	(No symbol) [0x00007FF68B8DF21F]
+	(No symbol) [0x00007FF68B8B6F33]
+	(No symbol) [0x00007FF68B880358]
+	(No symbol) [0x00007FF68B8810C3]
+	GetHandleVerifier [0x00007FF68BD3BAAD+3001437]
+	GetHandleVerifier [0x00007FF68BD35E92+2977858]
+	GetHandleVerifier [0x00007FF68BD5499D+3103565]
+	GetHandleVerifier [0x00007FF68BA8C81A+186826]
+	GetHandleVerifier [0x00007FF68BA9442F+218591]
+	GetHandleVerifier [0x00007FF68BA79DC4+110452]
+	GetHandleVerifier [0x00007FF68BA79F72+110882]
+	GetHandleVerifier [0x00007FF68BA603A9+5465]
+	BaseThreadInitThunk [0x00007FFD0A3EE8D7+23]
+	RtlUserThreadStart [0x00007FFD0B8DBF6C+44]
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-04-06 22:59:33</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>918849958013</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Image: 65322a94-e7e5-4b4e-b7e7-f0eea51b01de.jpg</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Message: 
+Stacktrace:
+	GetHandleVerifier [0x00007FF68BA71F85+78133]
+	GetHandleVerifier [0x00007FF68BA71FE0+78224]
+	(No symbol) [0x00007FF68B8391BA]
+	(No symbol) [0x00007FF68B88F19D]
+	(No symbol) [0x00007FF68B88F44C]
+	(No symbol) [0x00007FF68B8E23D7]
+	(No symbol) [0x00007FF68B8B719F]
+	(No symbol) [0x00007FF68B8DF21F]
+	(No symbol) [0x00007FF68B8B6F33]
+	(No symbol) [0x00007FF68B880358]
+	(No symbol) [0x00007FF68B8810C3]
+	GetHandleVerifier [0x00007FF68BD3BAAD+3001437]
+	GetHandleVerifier [0x00007FF68BD35E92+2977858]
+	GetHandleVerifier [0x00007FF68BD5499D+3103565]
+	GetHandleVerifier [0x00007FF68BA8C81A+186826]
+	GetHandleVerifier [0x00007FF68BA9442F+218591]
+	GetHandleVerifier [0x00007FF68BA79DC4+110452]
+	GetHandleVerifier [0x00007FF68BA79F72+110882]
+	GetHandleVerifier [0x00007FF68BA603A9+5465]
+	BaseThreadInitThunk [0x00007FFD0A3EE8D7+23]
+	RtlUserThreadStart [0x00007FFD0B8DBF6C+44]
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-04-06 23:03:34</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>918849958013</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Image: f41b2bcd-91ea-4c2b-8d38-af49c491fe4c.jpg</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Message: 
+Stacktrace:
+	GetHandleVerifier [0x00007FF68BA71F85+78133]
+	GetHandleVerifier [0x00007FF68BA71FE0+78224]
+	(No symbol) [0x00007FF68B8391BA]
+	(No symbol) [0x00007FF68B88F19D]
+	(No symbol) [0x00007FF68B88F44C]
+	(No symbol) [0x00007FF68B8E23D7]
+	(No symbol) [0x00007FF68B8B719F]
+	(No symbol) [0x00007FF68B8DF21F]
+	(No symbol) [0x00007FF68B8B6F33]
+	(No symbol) [0x00007FF68B880358]
+	(No symbol) [0x00007FF68B8810C3]
+	GetHandleVerifier [0x00007FF68BD3BAAD+3001437]
+	GetHandleVerifier [0x00007FF68BD35E92+2977858]
+	GetHandleVerifier [0x00007FF68BD5499D+3103565]
+	GetHandleVerifier [0x00007FF68BA8C81A+186826]
+	GetHandleVerifier [0x00007FF68BA9442F+218591]
+	GetHandleVerifier [0x00007FF68BA79DC4+110452]
+	GetHandleVerifier [0x00007FF68BA79F72+110882]
+	GetHandleVerifier [0x00007FF68BA603A9+5465]
+	BaseThreadInitThunk [0x00007FFD0A3EE8D7+23]
+	RtlUserThreadStart [0x00007FFD0B8DBF6C+44]
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-04-06 23:12:40</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>918849958013</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Image: e30546a7-5841-4a13-a08d-7460ec2eb101.png</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Message: 
+Stacktrace:
+	GetHandleVerifier [0x00007FF68BA71F85+78133]
+	GetHandleVerifier [0x00007FF68BA71FE0+78224]
+	(No symbol) [0x00007FF68B8391BA]
+	(No symbol) [0x00007FF68B88F19D]
+	(No symbol) [0x00007FF68B88F44C]
+	(No symbol) [0x00007FF68B8E23D7]
+	(No symbol) [0x00007FF68B8B719F]
+	(No symbol) [0x00007FF68B8DF21F]
+	(No symbol) [0x00007FF68B8B6F33]
+	(No symbol) [0x00007FF68B880358]
+	(No symbol) [0x00007FF68B8810C3]
+	GetHandleVerifier [0x00007FF68BD3BAAD+3001437]
+	GetHandleVerifier [0x00007FF68BD35E92+2977858]
+	GetHandleVerifier [0x00007FF68BD5499D+3103565]
+	GetHandleVerifier [0x00007FF68BA8C81A+186826]
+	GetHandleVerifier [0x00007FF68BA9442F+218591]
+	GetHandleVerifier [0x00007FF68BA79DC4+110452]
+	GetHandleVerifier [0x00007FF68BA79F72+110882]
+	GetHandleVerifier [0x00007FF68BA603A9+5465]
+	BaseThreadInitThunk [0x00007FFD0A3EE8D7+23]
+	RtlUserThreadStart [0x00007FFD0B8DBF6C+44]
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-04-06 23:17:51</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>918849958013</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>szxdcfbhnjmk</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-04-06 23:24:59</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>919284374259</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>sdfghjkl;</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-04-07 20:57:32</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>919322612069</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-04-07 20:57:45</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>916353481830</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-04-07 21:12:57</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>918849958013</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Hello John Doe!</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-04-07 21:13:09</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>919322612069</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Hello John Doe!</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-04-07 21:13:20</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>917020811776</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Hello John Doe!</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-04-07 21:13:32</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>919824237224</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Hello John Doe!</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-04-07 21:23:36</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>918849958013</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Hello Yash Adagale!</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-04-07 21:23:47</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>919322612069</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Hello Yash Adagale!</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-04-07 21:23:58</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>919824237224</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Hello Yash Adagale!</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-04-07 21:27:23</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>918849958013</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-04-07 21:27:35</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>919322612069</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-04-07 21:27:47</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>919824237224</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
functionality of fetching the phone number from the csv,xlsx is added
</commit_message>
<xml_diff>
--- a/message_tracking/message_log.xlsx
+++ b/message_tracking/message_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3559,10 +3559,8 @@
           <t>2025-04-07 21:27:47</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>919824237224</t>
-        </is>
+      <c r="B78" t="n">
+        <v>919824237224</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -3580,6 +3578,34 @@
         </is>
       </c>
       <c r="F78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-04-07 21:41:33</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>918849958013</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
image sending code is commented
</commit_message>
<xml_diff>
--- a/message_tracking/message_log.xlsx
+++ b/message_tracking/message_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3585,10 +3585,8 @@
           <t>2025-04-07 21:41:33</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>918849958013</t>
-        </is>
+      <c r="B79" t="n">
+        <v>918849958013</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -3606,6 +3604,34 @@
         </is>
       </c>
       <c r="F79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2025-04-08 15:06:00</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>+919049148862</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>